<commit_message>
exit game and saves
</commit_message>
<xml_diff>
--- a/cms/Variables.xlsx
+++ b/cms/Variables.xlsx
@@ -651,21 +651,12 @@
     <t>«BUTTON-PREORDER»</t>
   </si>
   <si>
-    <t>&lt;h3&gt;Level navigation&lt;/h3&gt;&lt;p&gt;Navigate to «GN:Load» by pressing the &lt;b&gt;lateral buttons&lt;/b&gt; beside the game screen. These buttons appear and disappear as needed.&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>NAV-LEVEL</t>
   </si>
   <si>
-    <t>a previously uncovered level</t>
-  </si>
-  <si>
     <t>NAV-SAVED</t>
   </si>
   <si>
-    <t>the previous saved points</t>
-  </si>
-  <si>
     <t>&lt;h2&gt;About «TITLE-BOLD»&lt;/h2&gt;</t>
   </si>
   <si>
@@ -966,9 +957,6 @@
     <t>TITLE-BY</t>
   </si>
   <si>
-    <t>«TITLE:Load» by «NAME» «YEAR:Load»</t>
-  </si>
-  <si>
     <t>BUTTON-SUBSCRIBE</t>
   </si>
   <si>
@@ -1042,6 +1030,18 @@
   </si>
   <si>
     <t>&lt;a href="https://twitter.com/leslodev" «BLANK»&gt;&lt;b&gt;Lucas LeSlo&lt;/b&gt;&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>«TITLE-BOLD» by «NAME» «YEAR:Load»</t>
+  </si>
+  <si>
+    <t>&lt;h3&gt;Level navigation&lt;/h3&gt;&lt;p&gt;The &lt;b&gt;lateral buttons&lt;/b&gt; beside the game screen (which appear and disappear as needed) let you navigate «GN:Load»&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">between the current and previously solved levels. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> to a previous checkpoint, or return to the most recent one. Please be aware that saving after going to a past checkpoint will erase your most recent checkpoint saves. </t>
   </si>
 </sst>
 </file>
@@ -2067,7 +2067,7 @@
         <v>104</v>
       </c>
       <c r="B2" s="2">
-        <v>2018</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -2168,10 +2168,10 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
@@ -2259,7 +2259,7 @@
         <v>126</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
@@ -2304,34 +2304,34 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
@@ -2352,10 +2352,10 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>315</v>
+        <v>337</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
@@ -2507,7 +2507,7 @@
         <v>152</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
@@ -2520,18 +2520,18 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="2" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
@@ -2542,7 +2542,7 @@
         <v>44</v>
       </c>
       <c r="C61" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
@@ -2555,10 +2555,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
@@ -2619,18 +2619,18 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
@@ -2691,18 +2691,18 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" s="2" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
@@ -2790,7 +2790,7 @@
         <v>173</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
@@ -2822,23 +2822,23 @@
         <v>68</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>210</v>
+        <v>338</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>212</v>
+        <v>339</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>214</v>
+        <v>340</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
@@ -2902,15 +2902,15 @@
         <v>77</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
@@ -2931,10 +2931,10 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
@@ -2942,7 +2942,7 @@
         <v>184</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
@@ -2966,7 +2966,7 @@
         <v>186</v>
       </c>
       <c r="B114" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="17.5" x14ac:dyDescent="0.35">
@@ -2990,7 +2990,7 @@
         <v>189</v>
       </c>
       <c r="B117" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
@@ -3006,7 +3006,7 @@
         <v>191</v>
       </c>
       <c r="B119" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
@@ -3038,7 +3038,7 @@
         <v>194</v>
       </c>
       <c r="B123" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
@@ -3062,15 +3062,15 @@
         <v>196</v>
       </c>
       <c r="B126" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="B127" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
@@ -3107,235 +3107,235 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B132" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B133" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B134" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B135" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B136" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B137" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B138" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B139" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B140" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B141" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B142" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B143" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B144" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B145" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B146" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B147" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B148" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B149" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C149" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D149" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="E149" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B150" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B151" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B152" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B153" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B154" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B155" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B156" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B157" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B158" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B159" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.35">
@@ -3348,98 +3348,98 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B161" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B162" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B163" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="B164" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B165" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B166" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B167" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B168" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B169" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="B170" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="B171" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B172" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>